<commit_message>
Deleted table number entry
</commit_message>
<xml_diff>
--- a/AD_NameList.xlsx
+++ b/AD_NameList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c22d98c1d7531019/Desktop/Wheel of fortune/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_2B59D2BFD3E0DB790F9B3311590040316065E974" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACB6E7CB-49A4-4164-B8A3-187E248E70A5}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_2B59D2BFD3E0DB790F9B3311590040316065E974" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E0FDAE6-8F2E-4775-9C69-4D7DC632C141}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -308,6 +308,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,7 +602,7 @@
   <dimension ref="A1:B70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>